<commit_message>
Update Documents P3/Tracability Link Matrix (1).xlsx
</commit_message>
<xml_diff>
--- a/Documents P3/Tracability Link Matrix (1).xlsx
+++ b/Documents P3/Tracability Link Matrix (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meetkumar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunny/Documents/GitHub/cs414-f18-001-stringCheese/Documents P3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{02775543-AA00-44DC-9B3B-214FA0EDA423}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33180610-86F8-C04F-B098-4A053F776056}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t>ChessBoard</t>
   </si>
@@ -77,17 +77,33 @@
   </si>
   <si>
     <t>UC12-Display Valid Moves</t>
+  </si>
+  <si>
+    <t>Not Implemente yet</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Wawati TC"/>
+      <family val="3"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="4">
@@ -99,13 +115,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -137,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -145,11 +161,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1310,16 +1328,16 @@
   <dimension ref="A1:IV14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" style="1" customWidth="1"/>
-    <col min="2" max="256" width="14.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" style="1" customWidth="1"/>
+    <col min="2" max="256" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1340,7 +1358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1355,7 +1373,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1370,7 +1388,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1387,7 +1405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1402,7 +1420,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1419,7 +1437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1434,7 +1452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1449,7 +1467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1464,7 +1482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1479,28 +1497,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="B11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
@@ -1517,24 +1535,275 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:256" s="10" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="B13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="9"/>
+      <c r="AI13" s="9"/>
+      <c r="AJ13" s="9"/>
+      <c r="AK13" s="9"/>
+      <c r="AL13" s="9"/>
+      <c r="AM13" s="9"/>
+      <c r="AN13" s="9"/>
+      <c r="AO13" s="9"/>
+      <c r="AP13" s="9"/>
+      <c r="AQ13" s="9"/>
+      <c r="AR13" s="9"/>
+      <c r="AS13" s="9"/>
+      <c r="AT13" s="9"/>
+      <c r="AU13" s="9"/>
+      <c r="AV13" s="9"/>
+      <c r="AW13" s="9"/>
+      <c r="AX13" s="9"/>
+      <c r="AY13" s="9"/>
+      <c r="AZ13" s="9"/>
+      <c r="BA13" s="9"/>
+      <c r="BB13" s="9"/>
+      <c r="BC13" s="9"/>
+      <c r="BD13" s="9"/>
+      <c r="BE13" s="9"/>
+      <c r="BF13" s="9"/>
+      <c r="BG13" s="9"/>
+      <c r="BH13" s="9"/>
+      <c r="BI13" s="9"/>
+      <c r="BJ13" s="9"/>
+      <c r="BK13" s="9"/>
+      <c r="BL13" s="9"/>
+      <c r="BM13" s="9"/>
+      <c r="BN13" s="9"/>
+      <c r="BO13" s="9"/>
+      <c r="BP13" s="9"/>
+      <c r="BQ13" s="9"/>
+      <c r="BR13" s="9"/>
+      <c r="BS13" s="9"/>
+      <c r="BT13" s="9"/>
+      <c r="BU13" s="9"/>
+      <c r="BV13" s="9"/>
+      <c r="BW13" s="9"/>
+      <c r="BX13" s="9"/>
+      <c r="BY13" s="9"/>
+      <c r="BZ13" s="9"/>
+      <c r="CA13" s="9"/>
+      <c r="CB13" s="9"/>
+      <c r="CC13" s="9"/>
+      <c r="CD13" s="9"/>
+      <c r="CE13" s="9"/>
+      <c r="CF13" s="9"/>
+      <c r="CG13" s="9"/>
+      <c r="CH13" s="9"/>
+      <c r="CI13" s="9"/>
+      <c r="CJ13" s="9"/>
+      <c r="CK13" s="9"/>
+      <c r="CL13" s="9"/>
+      <c r="CM13" s="9"/>
+      <c r="CN13" s="9"/>
+      <c r="CO13" s="9"/>
+      <c r="CP13" s="9"/>
+      <c r="CQ13" s="9"/>
+      <c r="CR13" s="9"/>
+      <c r="CS13" s="9"/>
+      <c r="CT13" s="9"/>
+      <c r="CU13" s="9"/>
+      <c r="CV13" s="9"/>
+      <c r="CW13" s="9"/>
+      <c r="CX13" s="9"/>
+      <c r="CY13" s="9"/>
+      <c r="CZ13" s="9"/>
+      <c r="DA13" s="9"/>
+      <c r="DB13" s="9"/>
+      <c r="DC13" s="9"/>
+      <c r="DD13" s="9"/>
+      <c r="DE13" s="9"/>
+      <c r="DF13" s="9"/>
+      <c r="DG13" s="9"/>
+      <c r="DH13" s="9"/>
+      <c r="DI13" s="9"/>
+      <c r="DJ13" s="9"/>
+      <c r="DK13" s="9"/>
+      <c r="DL13" s="9"/>
+      <c r="DM13" s="9"/>
+      <c r="DN13" s="9"/>
+      <c r="DO13" s="9"/>
+      <c r="DP13" s="9"/>
+      <c r="DQ13" s="9"/>
+      <c r="DR13" s="9"/>
+      <c r="DS13" s="9"/>
+      <c r="DT13" s="9"/>
+      <c r="DU13" s="9"/>
+      <c r="DV13" s="9"/>
+      <c r="DW13" s="9"/>
+      <c r="DX13" s="9"/>
+      <c r="DY13" s="9"/>
+      <c r="DZ13" s="9"/>
+      <c r="EA13" s="9"/>
+      <c r="EB13" s="9"/>
+      <c r="EC13" s="9"/>
+      <c r="ED13" s="9"/>
+      <c r="EE13" s="9"/>
+      <c r="EF13" s="9"/>
+      <c r="EG13" s="9"/>
+      <c r="EH13" s="9"/>
+      <c r="EI13" s="9"/>
+      <c r="EJ13" s="9"/>
+      <c r="EK13" s="9"/>
+      <c r="EL13" s="9"/>
+      <c r="EM13" s="9"/>
+      <c r="EN13" s="9"/>
+      <c r="EO13" s="9"/>
+      <c r="EP13" s="9"/>
+      <c r="EQ13" s="9"/>
+      <c r="ER13" s="9"/>
+      <c r="ES13" s="9"/>
+      <c r="ET13" s="9"/>
+      <c r="EU13" s="9"/>
+      <c r="EV13" s="9"/>
+      <c r="EW13" s="9"/>
+      <c r="EX13" s="9"/>
+      <c r="EY13" s="9"/>
+      <c r="EZ13" s="9"/>
+      <c r="FA13" s="9"/>
+      <c r="FB13" s="9"/>
+      <c r="FC13" s="9"/>
+      <c r="FD13" s="9"/>
+      <c r="FE13" s="9"/>
+      <c r="FF13" s="9"/>
+      <c r="FG13" s="9"/>
+      <c r="FH13" s="9"/>
+      <c r="FI13" s="9"/>
+      <c r="FJ13" s="9"/>
+      <c r="FK13" s="9"/>
+      <c r="FL13" s="9"/>
+      <c r="FM13" s="9"/>
+      <c r="FN13" s="9"/>
+      <c r="FO13" s="9"/>
+      <c r="FP13" s="9"/>
+      <c r="FQ13" s="9"/>
+      <c r="FR13" s="9"/>
+      <c r="FS13" s="9"/>
+      <c r="FT13" s="9"/>
+      <c r="FU13" s="9"/>
+      <c r="FV13" s="9"/>
+      <c r="FW13" s="9"/>
+      <c r="FX13" s="9"/>
+      <c r="FY13" s="9"/>
+      <c r="FZ13" s="9"/>
+      <c r="GA13" s="9"/>
+      <c r="GB13" s="9"/>
+      <c r="GC13" s="9"/>
+      <c r="GD13" s="9"/>
+      <c r="GE13" s="9"/>
+      <c r="GF13" s="9"/>
+      <c r="GG13" s="9"/>
+      <c r="GH13" s="9"/>
+      <c r="GI13" s="9"/>
+      <c r="GJ13" s="9"/>
+      <c r="GK13" s="9"/>
+      <c r="GL13" s="9"/>
+      <c r="GM13" s="9"/>
+      <c r="GN13" s="9"/>
+      <c r="GO13" s="9"/>
+      <c r="GP13" s="9"/>
+      <c r="GQ13" s="9"/>
+      <c r="GR13" s="9"/>
+      <c r="GS13" s="9"/>
+      <c r="GT13" s="9"/>
+      <c r="GU13" s="9"/>
+      <c r="GV13" s="9"/>
+      <c r="GW13" s="9"/>
+      <c r="GX13" s="9"/>
+      <c r="GY13" s="9"/>
+      <c r="GZ13" s="9"/>
+      <c r="HA13" s="9"/>
+      <c r="HB13" s="9"/>
+      <c r="HC13" s="9"/>
+      <c r="HD13" s="9"/>
+      <c r="HE13" s="9"/>
+      <c r="HF13" s="9"/>
+      <c r="HG13" s="9"/>
+      <c r="HH13" s="9"/>
+      <c r="HI13" s="9"/>
+      <c r="HJ13" s="9"/>
+      <c r="HK13" s="9"/>
+      <c r="HL13" s="9"/>
+      <c r="HM13" s="9"/>
+      <c r="HN13" s="9"/>
+      <c r="HO13" s="9"/>
+      <c r="HP13" s="9"/>
+      <c r="HQ13" s="9"/>
+      <c r="HR13" s="9"/>
+      <c r="HS13" s="9"/>
+      <c r="HT13" s="9"/>
+      <c r="HU13" s="9"/>
+      <c r="HV13" s="9"/>
+      <c r="HW13" s="9"/>
+      <c r="HX13" s="9"/>
+      <c r="HY13" s="9"/>
+      <c r="HZ13" s="9"/>
+      <c r="IA13" s="9"/>
+      <c r="IB13" s="9"/>
+      <c r="IC13" s="9"/>
+      <c r="ID13" s="9"/>
+      <c r="IE13" s="9"/>
+      <c r="IF13" s="9"/>
+      <c r="IG13" s="9"/>
+      <c r="IH13" s="9"/>
+      <c r="II13" s="9"/>
+      <c r="IJ13" s="9"/>
+      <c r="IK13" s="9"/>
+      <c r="IL13" s="9"/>
+      <c r="IM13" s="9"/>
+      <c r="IN13" s="9"/>
+      <c r="IO13" s="9"/>
+      <c r="IP13" s="9"/>
+      <c r="IQ13" s="9"/>
+      <c r="IR13" s="9"/>
+      <c r="IS13" s="9"/>
+      <c r="IT13" s="9"/>
+      <c r="IU13" s="9"/>
+      <c r="IV13" s="9"/>
     </row>
-    <row r="14" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1544,6 +1813,7 @@
       <c r="G14" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>